<commit_message>
scrum report aya jihad layla
</commit_message>
<xml_diff>
--- a/src/main/resources/iteration3_scrumReport_wolf.xlsx
+++ b/src/main/resources/iteration3_scrumReport_wolf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\MineSweeper_Wolf\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA223ED-EA4A-4A3F-B359-9069F8EF05EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9677872D-DB01-4B74-89DD-6FAFB4540754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="100">
   <si>
     <t>Iteration</t>
   </si>
@@ -41,6 +41,285 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Iteration03</t>
+  </si>
+  <si>
+    <t>Define How To Play requirements (Easy Mode)</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Product owner</t>
+  </si>
+  <si>
+    <t>Aya</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Plan step-by-step tutorial flow</t>
+  </si>
+  <si>
+    <t>Scrum master</t>
+  </si>
+  <si>
+    <t>Define game rules for tutorial (Easy Mode)</t>
+  </si>
+  <si>
+    <t>Design How To Play navigation (Prev / Next / Play / Stop)</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Build HowToPlayView.fxml</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Build HowToPlayBoardBuilder</t>
+  </si>
+  <si>
+    <t>Build HowToPlayController (core logic)</t>
+  </si>
+  <si>
+    <t>Implement demo game state (fake board)</t>
+  </si>
+  <si>
+    <t>Implement reveal empty + cascade logic</t>
+  </si>
+  <si>
+    <t>Implement flag logic (no turn switch)</t>
+  </si>
+  <si>
+    <t>Implement reveal number cell</t>
+  </si>
+  <si>
+    <t>Implement turn switching logic</t>
+  </si>
+  <si>
+    <t>Implement mine behavior (lose life)</t>
+  </si>
+  <si>
+    <t>Implement shared hearts bar</t>
+  </si>
+  <si>
+    <t>Implement stats bar (mines, flags, questions, surprises)</t>
+  </si>
+  <si>
+    <t>Implement reveal Question cell</t>
+  </si>
+  <si>
+    <t>Implement activate Question (separate action)</t>
+  </si>
+  <si>
+    <t>Implement Question popup (tutorial mode)</t>
+  </si>
+  <si>
+    <t>Implement Question result popup (all outcomes)</t>
+  </si>
+  <si>
+    <t>Implement Easy-mode question scoring logic</t>
+  </si>
+  <si>
+    <t>Implement activation cost logic</t>
+  </si>
+  <si>
+    <t>Implement reveal Surprise cell</t>
+  </si>
+  <si>
+    <t>Implement activate Surprise (separate action)</t>
+  </si>
+  <si>
+    <t>Implement Surprise tutorial popup (GOOD + BAD)</t>
+  </si>
+  <si>
+    <t>Implement used-cell behavior</t>
+  </si>
+  <si>
+    <t>Implement highlight system (cell / row / neighbors)</t>
+  </si>
+  <si>
+    <t>Implement Auto Play tutorial mode</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Block PREV/NEXT during popup (modal behavior)</t>
+  </si>
+  <si>
+    <t>UX consistency with real game</t>
+  </si>
+  <si>
+    <t>Bug fixing &amp; refactoring</t>
+  </si>
+  <si>
+    <t>Scope limited to Easy Mode tutorial</t>
+  </si>
+  <si>
+    <t>Rules aligned with real game mechanics</t>
+  </si>
+  <si>
+    <t>Implemented as sequential TourSteps</t>
+  </si>
+  <si>
+    <t>Supports manual and automatic navigation</t>
+  </si>
+  <si>
+    <t>Central controller for tutorial logic</t>
+  </si>
+  <si>
+    <t>Board state is predefined for consistency</t>
+  </si>
+  <si>
+    <t>Cascade counts as one action</t>
+  </si>
+  <si>
+    <t>Flags do not end the turn</t>
+  </si>
+  <si>
+    <t>Turn switches only after turn-ending actions</t>
+  </si>
+  <si>
+    <t>Shared heart is reduced</t>
+  </si>
+  <si>
+    <t>Reveal does not activate the question</t>
+  </si>
+  <si>
+    <t>Requires activation cost</t>
+  </si>
+  <si>
+    <t>Correct answer is highlighted</t>
+  </si>
+  <si>
+    <t>Shows all possible answer effects</t>
+  </si>
+  <si>
+    <t>Easy/Medium include 50% chance outcomes</t>
+  </si>
+  <si>
+    <t>Cost applied before result</t>
+  </si>
+  <si>
+    <t>Reveal does not activate the surprise</t>
+  </si>
+  <si>
+    <t>Fixed outcome in tutorial</t>
+  </si>
+  <si>
+    <t>Both outcomes shown for explanation</t>
+  </si>
+  <si>
+    <t>Dark overlay + disabled interaction</t>
+  </si>
+  <si>
+    <t>Visual guidance using overlay rectangles</t>
+  </si>
+  <si>
+    <t>Includes delays and auto-close popups</t>
+  </si>
+  <si>
+    <t>Popups are modal by design</t>
+  </si>
+  <si>
+    <t>Tutorial mirrors real gameplay rules</t>
+  </si>
+  <si>
+    <t>Minor logic and UI fixes</t>
+  </si>
+  <si>
+    <t>Replace text labels with icons in game status bar</t>
+  </si>
+  <si>
+    <t>Replaced textual labels (e.g., “mines left”, “questions left”, “surprises left”) with intuitive icons in the real game UI to improve clarity and consistency with the board design.</t>
+  </si>
+  <si>
+    <t>UI improvement: Pop up resizes dynamically according to text size</t>
+  </si>
+  <si>
+    <t>Implementing select mode feature in questions management screen</t>
+  </si>
+  <si>
+    <t>UX improvement: added refresh functionality to history screen</t>
+  </si>
+  <si>
+    <t>UX improvement: redefinind choices of cancel button in edit and add questions screens</t>
+  </si>
+  <si>
+    <t>UX improvement: added an exception handling when filter textfield is empty in history screen</t>
+  </si>
+  <si>
+    <t>UI improvement: applyied smooth fade transitions between screens</t>
+  </si>
+  <si>
+    <t>Cleaning code in parts of the controllers</t>
+  </si>
+  <si>
+    <t>Implementing Design Patterns after team discussion and decision making</t>
+  </si>
+  <si>
+    <t>Writing design patterns report</t>
+  </si>
+  <si>
+    <t>Adding new questions to questions.csv</t>
+  </si>
+  <si>
+    <t>Jihad</t>
+  </si>
+  <si>
+    <t>Implemented a Forgot Password workflow with secure OTP verification and password reset.</t>
+  </si>
+  <si>
+    <t>Layla</t>
+  </si>
+  <si>
+    <t>Fixed critical gameplay logic inconsistencies, including limiting flag usage correctly to a maximum of 3 per turn.</t>
+  </si>
+  <si>
+    <t>Refactored the main game controller into six focused classes, improving separation of concerns, maintainability, and testability.</t>
+  </si>
+  <si>
+    <t>Resolved UI inconsistencies caused by mixed dialog and theme handling, ensuring consistent visual behavior across themes.</t>
+  </si>
+  <si>
+    <t>Centralized dialog creation and behavior into a reusable Dialog Utility, reducing duplication across controllers.</t>
+  </si>
+  <si>
+    <t>Refactored dialog-related logic out of controllers to improve software engineering quality.</t>
+  </si>
+  <si>
+    <t>Improved in-game popup clarity, especially for surprise and question popups</t>
+  </si>
+  <si>
+    <t>Refined login user experience with password visibility toggles, validation feedback, and input length limits.</t>
+  </si>
+  <si>
+    <t>Introduced guided onboarding for the Login screen to improve first-time user experience.</t>
+  </si>
+  <si>
+    <t>Implemented conditional visibility for the Login button, dynamically hiding it after login and restoring it when login is skipped.</t>
+  </si>
+  <si>
+    <t>Introduced guided onboarding for the New Game screen to improve usability.</t>
+  </si>
+  <si>
+    <t>Introduced guided onboarding for the Game screen to guide players during gameplay.</t>
+  </si>
+  <si>
+    <t>Cleaned up multiple controller classes to better align with software engineering and quality assurance standards.</t>
+  </si>
+  <si>
+    <t>Designed and implemented the initial customization infrastructure, establishing the foundation that was later extended by Adan.</t>
+  </si>
+  <si>
+    <t>Introduced guided onboarding for the History screen to improve usability.</t>
   </si>
 </sst>
 </file>
@@ -517,14 +796,14 @@
   <dimension ref="A1:I1011"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.09765625" customWidth="1"/>
-    <col min="2" max="2" width="44.19921875" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" customWidth="1"/>
+    <col min="2" max="2" width="73.3984375" customWidth="1"/>
     <col min="3" max="3" width="14.59765625" customWidth="1"/>
     <col min="4" max="4" width="17.8984375" customWidth="1"/>
     <col min="5" max="5" width="15.59765625" customWidth="1"/>
@@ -559,515 +838,1221 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
+      <c r="A11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
+      <c r="A13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
+      <c r="A14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="A15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="A16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
+      <c r="A17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
+      <c r="A18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
+      <c r="A19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
+      <c r="A20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
+      <c r="A21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7"/>
+      <c r="A22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
+      <c r="A23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7"/>
+      <c r="A24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
+      <c r="A25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="7"/>
+      <c r="A26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="7"/>
+      <c r="A27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="7"/>
+      <c r="A28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
+      <c r="A29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
+      <c r="A30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
+      <c r="A31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="7"/>
+      <c r="A32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
+      <c r="A33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+      <c r="D34" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
+      <c r="D35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
+      <c r="D36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
+      <c r="D37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
+      <c r="D38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="D39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
+      <c r="D40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="D41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
+      <c r="D42" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
+      <c r="A43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
+      <c r="A44" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
+      <c r="A45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
+      <c r="A46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
+      <c r="A47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
+      <c r="A48" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="A49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
+      <c r="A50" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
+      <c r="A51" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
+      <c r="A52" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
+      <c r="A53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
+      <c r="A54" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G54" s="7"/>
     </row>
     <row r="55" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
+      <c r="A55" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
+      <c r="A56" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G56" s="7"/>
     </row>
     <row r="57" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
+      <c r="A57" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G57" s="7"/>
     </row>
     <row r="58" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
+      <c r="A58" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B58" s="7"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -1076,7 +2061,9 @@
       <c r="G58" s="7"/>
     </row>
     <row r="59" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
+      <c r="A59" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B59" s="7"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
@@ -1085,7 +2072,9 @@
       <c r="G59" s="7"/>
     </row>
     <row r="60" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
+      <c r="A60" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B60" s="7"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -1094,7 +2083,9 @@
       <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
+      <c r="A61" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B61" s="7"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
@@ -1103,7 +2094,9 @@
       <c r="G61" s="7"/>
     </row>
     <row r="62" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
+      <c r="A62" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B62" s="7"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
@@ -1112,7 +2105,9 @@
       <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
+      <c r="A63" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B63" s="7"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
@@ -1121,7 +2116,9 @@
       <c r="G63" s="7"/>
     </row>
     <row r="64" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
+      <c r="A64" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B64" s="7"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
@@ -1130,7 +2127,9 @@
       <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
+      <c r="A65" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B65" s="7"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
@@ -1139,7 +2138,9 @@
       <c r="G65" s="7"/>
     </row>
     <row r="66" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
+      <c r="A66" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B66" s="7"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
@@ -1148,7 +2149,9 @@
       <c r="G66" s="7"/>
     </row>
     <row r="67" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
+      <c r="A67" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B67" s="7"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
@@ -1157,7 +2160,9 @@
       <c r="G67" s="7"/>
     </row>
     <row r="68" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
+      <c r="A68" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B68" s="7"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
@@ -1166,7 +2171,9 @@
       <c r="G68" s="7"/>
     </row>
     <row r="69" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
+      <c r="A69" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B69" s="7"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
@@ -1175,7 +2182,9 @@
       <c r="G69" s="7"/>
     </row>
     <row r="70" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
+      <c r="A70" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B70" s="7"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
@@ -1184,7 +2193,9 @@
       <c r="G70" s="7"/>
     </row>
     <row r="71" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
+      <c r="A71" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B71" s="7"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
@@ -9086,7 +10097,7 @@
     <row r="1011" ht="13.8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="B2:B939 G2:G939" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="B33:B939 B2 B5:B15 B17 B19 B21:B22 G2:G8 G12:G13 G15:G16 G33:G939" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation type="list" allowBlank="1" sqref="C2:C939" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"P1,P2,P3"</formula1>
     </dataValidation>

</xml_diff>